<commit_message>
changes related to update using id
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghous\Desktop\GigForce\excel_upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339C1676-5288-4BEB-9E44-7DEC81F623A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAE5396-8967-41B1-A783-235B72D1C5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2720" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>name</t>
   </si>
@@ -39,9 +39,6 @@
     <t>saman</t>
   </si>
   <si>
-    <t>tt</t>
-  </si>
-  <si>
     <t>rahul</t>
   </si>
   <si>
@@ -52,6 +49,12 @@
   </si>
   <si>
     <t>games</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>table tennis</t>
   </si>
 </sst>
 </file>
@@ -369,56 +372,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="C4">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>